<commit_message>
Warnings if some industry has mandatory inputs not settled
</commit_message>
<xml_diff>
--- a/dist/wiat_locations.xlsx
+++ b/dist/wiat_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PhpstormProjects\wiat_front\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3637F3C9-3698-4056-BD31-1842C65632D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6131B01D-F360-4A27-8564-AA44BF481A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{60B8F55B-90B2-41A0-953E-FD593A0D51DC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Latitude</t>
   </si>
@@ -76,13 +76,24 @@
   </si>
   <si>
     <t>Add as many suppliers (Name, Latitude, Longitude) as needed to the right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTRUCTIONS: </t>
+  </si>
+  <si>
+    <t>Add the assessments you want to add to the tool on the first sheet.
+ If the name of any assessment coincides with an existing one, the latter (along with its industries) will be deleted.</t>
+  </si>
+  <si>
+    <t>In the industries tab, define the industries you want to add, together 
+with the assessment to which it belongs. This assessment does not have to be defined in the assessment sheet, it can be previously defined in the web tool.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +111,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -190,6 +209,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -197,7 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,6 +293,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -553,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155DBE8A-0346-4315-8D01-639509365F15}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,26 +632,26 @@
     <col min="2" max="2" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="13.08984375" customWidth="1"/>
     <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="57.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -595,9 +662,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -605,6 +685,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>